<commit_message>
Updating structure of all test fixtures for integration tests. Now working.
</commit_message>
<xml_diff>
--- a/tests/fixtures/constants/input_data/input_data.xlsx
+++ b/tests/fixtures/constants/input_data/input_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\default\0_constants\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\fixtures\constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8D70C3-1AB9-4B50-AE67-4D3BAFB2196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8FDCB7-4A8F-482C-986F-148A9EEFE563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34820" yWindow="3610" windowWidth="15360" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32180" yWindow="2500" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q" sheetId="1" r:id="rId1"/>
@@ -415,7 +415,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -462,7 +462,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -490,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -504,7 +504,7 @@
         <v>9</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>